<commit_message>
udpate spreadsheet column names
</commit_message>
<xml_diff>
--- a/analysis/data/Supplementary_Information/KWL_excavation_depth.xlsx
+++ b/analysis/data/Supplementary_Information/KWL_excavation_depth.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/EmilyWang/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/EmilyWang/Desktop/School document/LW-Paper/kwl-ornaments-2019/analysis/data/Supplementary_Information/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7F0090B-CF97-4E4E-95F8-B5260DA8C040}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0022A570-1C5D-8E4F-A27F-C5EBEF3A6F7D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="780" yWindow="960" windowWidth="27640" windowHeight="16060" xr2:uid="{E5A116E0-62B6-7E4B-939F-078D4BD98D45}"/>
   </bookViews>
@@ -468,7 +468,7 @@
     <t>AT2P9</t>
   </si>
   <si>
-    <t>Trench</t>
+    <t>Unit_old</t>
   </si>
 </sst>
 </file>

</xml_diff>